<commit_message>
adds first draft of chapter 6
</commit_message>
<xml_diff>
--- a/mockups/Konkurrenzdarstellung.xlsx
+++ b/mockups/Konkurrenzdarstellung.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>GitFit</t>
   </si>
@@ -57,6 +57,12 @@
   </si>
   <si>
     <t>Zusatzfunktionen</t>
+  </si>
+  <si>
+    <t>myClub</t>
+  </si>
+  <si>
+    <t>technogym</t>
   </si>
 </sst>
 </file>
@@ -201,7 +207,7 @@
           <c:spPr>
             <a:ln w="28575" cap="rnd">
               <a:solidFill>
-                <a:schemeClr val="accent1"/>
+                <a:srgbClr val="C00000"/>
               </a:solidFill>
               <a:round/>
             </a:ln>
@@ -294,7 +300,10 @@
           <c:spPr>
             <a:ln w="28575" cap="rnd">
               <a:solidFill>
-                <a:schemeClr val="accent2"/>
+                <a:schemeClr val="accent4">
+                  <a:lumMod val="40000"/>
+                  <a:lumOff val="60000"/>
+                </a:schemeClr>
               </a:solidFill>
               <a:round/>
             </a:ln>
@@ -370,6 +379,198 @@
           </c:val>
           <c:smooth val="0"/>
         </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$D$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>myClub</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2">
+                  <a:lumMod val="40000"/>
+                  <a:lumOff val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$A$2:$A$9</c:f>
+              <c:strCache>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>Qualität</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Preis</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Leistung</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Handhabung</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Prestige</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Umweltfreundlichkeit</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Design</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Zusatzfunktionen</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$D$2:$D$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>4.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>5.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>6.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$E$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>technogym</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent6">
+                  <a:lumMod val="40000"/>
+                  <a:lumOff val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$A$2:$A$9</c:f>
+              <c:strCache>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>Qualität</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Preis</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Leistung</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Handhabung</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Prestige</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Umweltfreundlichkeit</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Design</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Zusatzfunktionen</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$E$2:$E$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>5.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>4.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>5.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
           <c:showVal val="0"/>
@@ -379,11 +580,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="-352865872"/>
-        <c:axId val="-402846064"/>
+        <c:axId val="655477984"/>
+        <c:axId val="655482656"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-352865872"/>
+        <c:axId val="655477984"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -426,7 +627,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-402846064"/>
+        <c:crossAx val="655482656"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -434,7 +635,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-402846064"/>
+        <c:axId val="655482656"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -484,7 +685,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-352865872"/>
+        <c:crossAx val="655477984"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1127,8 +1328,8 @@
     <xdr:from>
       <xdr:col>6</xdr:col>
       <xdr:colOff>76200</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>12700</xdr:rowOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>177800</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
@@ -1419,10 +1620,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C9"/>
+  <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1430,15 +1631,21 @@
     <col min="1" max="1" width="19.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B1" t="s">
         <v>0</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
       </c>
+      <c r="D1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1" t="s">
+        <v>11</v>
+      </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -1448,8 +1655,14 @@
       <c r="C2">
         <v>5</v>
       </c>
+      <c r="D2">
+        <v>4</v>
+      </c>
+      <c r="E2">
+        <v>5</v>
+      </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -1459,8 +1672,14 @@
       <c r="C3">
         <v>7</v>
       </c>
+      <c r="D3">
+        <v>4</v>
+      </c>
+      <c r="E3">
+        <v>6</v>
+      </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -1470,8 +1689,14 @@
       <c r="C4">
         <v>5</v>
       </c>
+      <c r="D4">
+        <v>4</v>
+      </c>
+      <c r="E4">
+        <v>5</v>
+      </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -1481,8 +1706,14 @@
       <c r="C5">
         <v>6</v>
       </c>
+      <c r="D5">
+        <v>5</v>
+      </c>
+      <c r="E5">
+        <v>4</v>
+      </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -1492,8 +1723,14 @@
       <c r="C6">
         <v>5</v>
       </c>
+      <c r="D6">
+        <v>3</v>
+      </c>
+      <c r="E6">
+        <v>4</v>
+      </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>7</v>
       </c>
@@ -1503,8 +1740,14 @@
       <c r="C7">
         <v>3</v>
       </c>
+      <c r="D7">
+        <v>5</v>
+      </c>
+      <c r="E7">
+        <v>4</v>
+      </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>8</v>
       </c>
@@ -1514,8 +1757,14 @@
       <c r="C8">
         <v>7</v>
       </c>
+      <c r="D8">
+        <v>5</v>
+      </c>
+      <c r="E8">
+        <v>6</v>
+      </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>9</v>
       </c>
@@ -1524,6 +1773,12 @@
       </c>
       <c r="C9">
         <v>3</v>
+      </c>
+      <c r="D9">
+        <v>6</v>
+      </c>
+      <c r="E9">
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
minor changes in chapter 7
</commit_message>
<xml_diff>
--- a/mockups/Konkurrenzdarstellung.xlsx
+++ b/mockups/Konkurrenzdarstellung.xlsx
@@ -255,19 +255,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>4.0</c:v>
+                  <c:v>6.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>5.0</c:v>
+                  <c:v>7.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>5.0</c:v>
+                  <c:v>6.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>7.0</c:v>
+                  <c:v>6.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>4.0</c:v>
+                  <c:v>3.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>6.0</c:v>
@@ -276,7 +276,7 @@
                   <c:v>7.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>5.0</c:v>
+                  <c:v>4.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -353,7 +353,7 @@
                   <c:v>5.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>7.0</c:v>
+                  <c:v>4.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>5.0</c:v>
@@ -448,7 +448,7 @@
                   <c:v>4.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4.0</c:v>
+                  <c:v>5.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>4.0</c:v>
@@ -543,7 +543,7 @@
                   <c:v>5.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>6.0</c:v>
+                  <c:v>3.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>5.0</c:v>
@@ -1632,7 +1632,7 @@
   <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G30" sqref="G30"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1659,7 +1659,7 @@
         <v>2</v>
       </c>
       <c r="B2">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C2">
         <v>5</v>
@@ -1676,16 +1676,16 @@
         <v>3</v>
       </c>
       <c r="B3">
+        <v>7</v>
+      </c>
+      <c r="C3">
+        <v>4</v>
+      </c>
+      <c r="D3">
         <v>5</v>
       </c>
-      <c r="C3">
-        <v>7</v>
-      </c>
-      <c r="D3">
-        <v>4</v>
-      </c>
       <c r="E3">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
@@ -1693,7 +1693,7 @@
         <v>4</v>
       </c>
       <c r="B4">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C4">
         <v>5</v>
@@ -1710,7 +1710,7 @@
         <v>5</v>
       </c>
       <c r="B5">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C5">
         <v>6</v>
@@ -1727,7 +1727,7 @@
         <v>6</v>
       </c>
       <c r="B6">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C6">
         <v>5</v>
@@ -1778,7 +1778,7 @@
         <v>9</v>
       </c>
       <c r="B9">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C9">
         <v>3</v>

</xml_diff>